<commit_message>
1.Created a new package for the latest test scripts and XML files - 'mainAppFlow'.
2. Developed a new test - VerReq_AddSmartFormItem_PerformCheckOut().
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/SmartForm.xlsx
+++ b/src/test/resources/datasheets/SmartForm.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -427,11 +427,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Created a new page class and added the following methods in Invoices page: 1.clickInvoices 2.clickbtnCreateNewInvoice. 3.selectPurchaseOrderToCreateInvoice(PO_Number). 4.selectItemToCreateInvoice,and 5.createMemoAndSubmitInvoice(PO_Number).
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/SmartForm.xlsx
+++ b/src/test/resources/datasheets/SmartForm.xlsx
@@ -427,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>